<commit_message>
all changes done to test.py and excel sheet. plz check
</commit_message>
<xml_diff>
--- a/Stud_Details.xlsx
+++ b/Stud_Details.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lakshya Sharma\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -81,13 +76,28 @@
   </si>
   <si>
     <t>Pranath Amma</t>
+  </si>
+  <si>
+    <t>Sidhartha Nambiar</t>
+  </si>
+  <si>
+    <t>1MS16CS044</t>
+  </si>
+  <si>
+    <t>nambiar.sidhartha00@gmail.com</t>
+  </si>
+  <si>
+    <t>Sidhrtha Appa</t>
+  </si>
+  <si>
+    <t>Sidhartha Amma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,31 +420,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -510,14 +520,41 @@
       </c>
       <c r="H3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>8848779798</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>